<commit_message>
Lab 6, ex 1 with Tomusca Raul
</commit_message>
<xml_diff>
--- a/Teodora_Rabagel/Lab4.xlsx
+++ b/Teodora_Rabagel/Lab4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FacultateTeo\an 4\sem1\SOAC\Laborator\SOAC_23-24\Teodora_Rabagel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FacultateTeo\an 4\sem1\SOAC\_Laborator\SOAC_23-24\Teodora_Rabagel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0797E6C2-83F3-4278-843B-1AFDB8E1B1C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C956C1-C6B0-43F2-82CC-A2E31175C275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1044" yWindow="1656" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3075" yWindow="3210" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -454,17 +454,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.21875" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -472,22 +472,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -495,7 +495,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -524,7 +524,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -553,7 +553,7 @@
         <v>0.40329999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -582,7 +582,7 @@
         <v>0.48930000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -611,7 +611,7 @@
         <v>0.50180000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -640,7 +640,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -677,7 +677,7 @@
         <v>37.18</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -714,7 +714,7 @@
         <v>14.989999999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -751,7 +751,7 @@
         <v>10.290000000000006</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -759,7 +759,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -788,7 +788,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -817,7 +817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -846,7 +846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -875,7 +875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -883,7 +883,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -912,7 +912,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -941,7 +941,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -970,7 +970,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -999,7 +999,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1010,7 +1010,7 @@
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -1047,22 +1047,22 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>2</v>
       </c>
@@ -1091,22 +1091,22 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>30</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>2</v>
       </c>
@@ -1143,22 +1143,22 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>29</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>2</v>
       </c>
@@ -1195,17 +1195,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>26</v>
       </c>

</xml_diff>